<commit_message>
Updated USA_grids model - 2025-08-22 20:09
</commit_message>
<xml_diff>
--- a/VerveStacks_USA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
+++ b/VerveStacks_USA_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62251D92-A7A1-4E41-9321-DC8AFAF1B067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2E85516-1069-48F9-942C-F8BFB6781012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,7 +618,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9111DB2F-A066-D271-766A-A1B927AD09DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{346D8AFC-20D8-FB15-CE6A-47B028D01437}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>